<commit_message>
Atualização Mapeamento ETL - Novo Servidor
</commit_message>
<xml_diff>
--- a/Documentação/Migração Servidores/Cosmos003/Mapeamento ETL.xlsx
+++ b/Documentação/Migração Servidores/Cosmos003/Mapeamento ETL.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10469" uniqueCount="3427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10513" uniqueCount="3436">
   <si>
     <t>Job</t>
   </si>
@@ -10300,6 +10300,33 @@
   </si>
   <si>
     <t>Precisamos adaptar a configuração do Excel para 32 bits e rever as conexões com a saída dos dados para Excel</t>
+  </si>
+  <si>
+    <t>Existe um "Script Task" que envia e-mail. Precisa ser revisto. Precisamos revisar também se todas as variáveis definidas são realmente utilizadas</t>
+  </si>
+  <si>
+    <t>verificar as variáveis de conexão.</t>
+  </si>
+  <si>
+    <t>O Banco MIS_LN não existe neste diretorio</t>
+  </si>
+  <si>
+    <t>O banco DM_MARKETING não existe no servidor. Precisamos adaptar a configuração do Excel para 32 bits</t>
+  </si>
+  <si>
+    <t>Existe um "Script Task" que envia e-mails.</t>
+  </si>
+  <si>
+    <t>Revisado?</t>
+  </si>
+  <si>
+    <t>Precisamos configurar o "SharePoint List Source"</t>
+  </si>
+  <si>
+    <t>precisamos reconfigurar na tabela adm.ssis_conexoes o OLAP</t>
+  </si>
+  <si>
+    <t>Em Package Configuration existe a leitura "Config FTP", porém não encontrei onde a mesma é utilizada. Em connection manager existe "File to Send" que também não encontrei onde é utilizado.</t>
   </si>
 </sst>
 </file>
@@ -10441,7 +10468,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -10484,14 +10511,41 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="26">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -10884,36 +10938,38 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela4" displayName="Tabela4" ref="A1:C183" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
-  <autoFilter ref="A1:C183">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela4" displayName="Tabela4" ref="A1:D183" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+  <autoFilter ref="A1:D183">
     <filterColumn colId="2"/>
+    <filterColumn colId="3"/>
   </autoFilter>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Diretorio " dataDxfId="22"/>
-    <tableColumn id="2" name="Job associado?" dataDxfId="21"/>
-    <tableColumn id="3" name="Observação" dataDxfId="20"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Diretorio " dataDxfId="23"/>
+    <tableColumn id="2" name="Job associado?" dataDxfId="22"/>
+    <tableColumn id="4" name="Revisado?" dataDxfId="0"/>
+    <tableColumn id="3" name="Observação" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A6:G1404" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A6:G1404" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <tableColumns count="7">
-    <tableColumn id="1" name="Job" dataDxfId="17"/>
-    <tableColumn id="2" name="step_name" dataDxfId="16"/>
-    <tableColumn id="3" name="Comando" dataDxfId="15"/>
-    <tableColumn id="4" name="Revisado" dataDxfId="14"/>
-    <tableColumn id="6" name="Alterado" dataDxfId="13"/>
-    <tableColumn id="5" name="Observação" dataDxfId="12"/>
-    <tableColumn id="7" name="Alteração após 18/09" dataDxfId="11"/>
+    <tableColumn id="1" name="Job" dataDxfId="18"/>
+    <tableColumn id="2" name="step_name" dataDxfId="17"/>
+    <tableColumn id="3" name="Comando" dataDxfId="16"/>
+    <tableColumn id="4" name="Revisado" dataDxfId="15"/>
+    <tableColumn id="6" name="Alterado" dataDxfId="14"/>
+    <tableColumn id="5" name="Observação" dataDxfId="13"/>
+    <tableColumn id="7" name="Alteração após 18/09" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela14" displayName="Tabela14" ref="A6:C329" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela14" displayName="Tabela14" ref="A6:C329" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A6:C329">
     <filterColumn colId="1">
       <filters>
@@ -10927,25 +10983,25 @@
     <sortCondition ref="B7:B848"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" name="Job" dataDxfId="8"/>
-    <tableColumn id="3" name="Diretorio" dataDxfId="7"/>
-    <tableColumn id="4" name="Revisado" dataDxfId="6"/>
+    <tableColumn id="1" name="Job" dataDxfId="9"/>
+    <tableColumn id="3" name="Diretorio" dataDxfId="8"/>
+    <tableColumn id="4" name="Revisado" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabela16" displayName="Tabela16" ref="A6:D837" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabela16" displayName="Tabela16" ref="A6:D837" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A6:D837"/>
   <sortState ref="A7:D837">
     <sortCondition ref="A7:A837"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="6" name="Solução" dataDxfId="3"/>
-    <tableColumn id="1" name="Job" dataDxfId="2"/>
-    <tableColumn id="2" name="step_name" dataDxfId="1"/>
-    <tableColumn id="7" name="Dtsx" dataDxfId="0"/>
+    <tableColumn id="6" name="Solução" dataDxfId="4"/>
+    <tableColumn id="1" name="Job" dataDxfId="3"/>
+    <tableColumn id="2" name="step_name" dataDxfId="2"/>
+    <tableColumn id="7" name="Dtsx" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -11236,1670 +11292,1692 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C183"/>
+  <dimension ref="A1:D183"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="45" style="8" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="16" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="8"/>
+    <col min="2" max="2" width="18.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="10" customFormat="1" ht="15">
+    <row r="1" spans="1:4" s="10" customFormat="1" ht="15">
       <c r="A1" s="9" t="s">
         <v>2623</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>2626</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="6" t="s">
+        <v>3432</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>3393</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" s="8" t="s">
         <v>2444</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C2" s="11"/>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="C2" s="7" t="s">
+        <v>2247</v>
+      </c>
+      <c r="D2" s="11"/>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="8" t="s">
         <v>2246</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C3" s="11"/>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="C3" s="7" t="s">
+        <v>2247</v>
+      </c>
+      <c r="D3" s="11"/>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="8" t="s">
         <v>2445</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C4" s="11"/>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="C4" s="7" t="s">
+        <v>2247</v>
+      </c>
+      <c r="D4" s="11"/>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="8" t="s">
         <v>2446</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C5" s="11"/>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="C5" s="7" t="s">
+        <v>2247</v>
+      </c>
+      <c r="D5" s="11"/>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="8" t="s">
         <v>2447</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C6" s="11"/>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="C6" s="7" t="s">
+        <v>2247</v>
+      </c>
+      <c r="D6" s="11"/>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="8" t="s">
         <v>2448</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>2625</v>
       </c>
-      <c r="C7" s="11"/>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" s="11"/>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="8" t="s">
         <v>2449</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>2625</v>
       </c>
-      <c r="C8" s="11"/>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8" s="11"/>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="8" t="s">
         <v>2450</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C9" s="11"/>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="C9" s="7" t="s">
+        <v>2247</v>
+      </c>
+      <c r="D9" s="11"/>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="8" t="s">
         <v>2451</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C10" s="11"/>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10" s="11"/>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="8" t="s">
         <v>2452</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C11" s="11"/>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="D11" s="11"/>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="8" t="s">
         <v>2453</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>2625</v>
       </c>
-      <c r="C12" s="11"/>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="D12" s="11"/>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="8" t="s">
         <v>2454</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C13" s="11"/>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="D13" s="11"/>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="8" t="s">
         <v>2455</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C14" s="11"/>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="D14" s="11"/>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="8" t="s">
         <v>2456</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C15" s="11"/>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="D15" s="11"/>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="8" t="s">
         <v>2457</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C16" s="11"/>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16" s="11"/>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="8" t="s">
         <v>2458</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C17" s="11"/>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17" s="11"/>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="8" t="s">
         <v>2459</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C18" s="11"/>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="D18" s="11"/>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="8" t="s">
         <v>2460</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C19" s="11"/>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="D19" s="11"/>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="8" t="s">
         <v>2461</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C20" s="11"/>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="D20" s="11"/>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="8" t="s">
         <v>2462</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C21" s="11"/>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="D21" s="11"/>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" s="8" t="s">
         <v>2463</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C22" s="11"/>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="D22" s="11"/>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" s="8" t="s">
         <v>2464</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C23" s="11"/>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="D23" s="11"/>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" s="8" t="s">
         <v>2465</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C24" s="11"/>
-    </row>
-    <row r="25" spans="1:3">
+      <c r="D24" s="11"/>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" s="8" t="s">
         <v>2466</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>2625</v>
       </c>
-      <c r="C25" s="11"/>
-    </row>
-    <row r="26" spans="1:3">
+      <c r="D25" s="11"/>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" s="8" t="s">
         <v>2467</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C26" s="11"/>
-    </row>
-    <row r="27" spans="1:3">
+      <c r="D26" s="11"/>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" s="8" t="s">
         <v>2468</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C27" s="11"/>
-    </row>
-    <row r="28" spans="1:3">
+      <c r="D27" s="11"/>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" s="8" t="s">
         <v>2469</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C28" s="11"/>
-    </row>
-    <row r="29" spans="1:3">
+      <c r="D28" s="11"/>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" s="8" t="s">
         <v>2470</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C29" s="11"/>
-    </row>
-    <row r="30" spans="1:3">
+      <c r="D29" s="11"/>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" s="8" t="s">
         <v>2471</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C30" s="11"/>
-    </row>
-    <row r="31" spans="1:3">
+      <c r="D30" s="11"/>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" s="8" t="s">
         <v>2472</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>2625</v>
       </c>
-      <c r="C31" s="11"/>
-    </row>
-    <row r="32" spans="1:3">
+      <c r="D31" s="11"/>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" s="8" t="s">
         <v>2473</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>2625</v>
       </c>
-      <c r="C32" s="11"/>
-    </row>
-    <row r="33" spans="1:3">
+      <c r="D32" s="11"/>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33" s="8" t="s">
         <v>2474</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>2625</v>
       </c>
-      <c r="C33" s="11"/>
-    </row>
-    <row r="34" spans="1:3">
+      <c r="D33" s="11"/>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" s="8" t="s">
         <v>2475</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>2625</v>
       </c>
-      <c r="C34" s="11"/>
-    </row>
-    <row r="35" spans="1:3">
+      <c r="D34" s="11"/>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35" s="8" t="s">
         <v>2476</v>
       </c>
       <c r="B35" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C35" s="11"/>
-    </row>
-    <row r="36" spans="1:3">
+      <c r="D35" s="11"/>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" s="8" t="s">
         <v>2477</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C36" s="11"/>
-    </row>
-    <row r="37" spans="1:3">
+      <c r="D36" s="11"/>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37" s="8" t="s">
         <v>2478</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>2625</v>
       </c>
-      <c r="C37" s="11"/>
-    </row>
-    <row r="38" spans="1:3">
+      <c r="D37" s="11"/>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" s="8" t="s">
         <v>2479</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>2625</v>
       </c>
-      <c r="C38" s="11"/>
-    </row>
-    <row r="39" spans="1:3">
+      <c r="D38" s="11"/>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39" s="8" t="s">
         <v>2480</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C39" s="11"/>
-    </row>
-    <row r="40" spans="1:3">
+      <c r="D39" s="11"/>
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40" s="8" t="s">
         <v>2481</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C40" s="11"/>
-    </row>
-    <row r="41" spans="1:3">
+      <c r="D40" s="11"/>
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41" s="8" t="s">
         <v>2482</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>2625</v>
       </c>
-      <c r="C41" s="11"/>
-    </row>
-    <row r="42" spans="1:3">
+      <c r="D41" s="11"/>
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42" s="8" t="s">
         <v>2483</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C42" s="11"/>
-    </row>
-    <row r="43" spans="1:3">
+      <c r="D42" s="11"/>
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43" s="8" t="s">
         <v>2484</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C43" s="11"/>
-    </row>
-    <row r="44" spans="1:3">
+      <c r="D43" s="11"/>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44" s="8" t="s">
         <v>2485</v>
       </c>
       <c r="B44" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C44" s="11"/>
-    </row>
-    <row r="45" spans="1:3">
+      <c r="D44" s="11"/>
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45" s="8" t="s">
         <v>2486</v>
       </c>
       <c r="B45" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C45" s="11"/>
-    </row>
-    <row r="46" spans="1:3">
+      <c r="D45" s="11"/>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46" s="8" t="s">
         <v>2487</v>
       </c>
       <c r="B46" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C46" s="11"/>
-    </row>
-    <row r="47" spans="1:3">
+      <c r="D46" s="11"/>
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47" s="8" t="s">
         <v>2488</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>2625</v>
       </c>
-      <c r="C47" s="11"/>
-    </row>
-    <row r="48" spans="1:3">
+      <c r="D47" s="11"/>
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48" s="8" t="s">
         <v>2489</v>
       </c>
       <c r="B48" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C48" s="11"/>
-    </row>
-    <row r="49" spans="1:3">
+      <c r="D48" s="11"/>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49" s="8" t="s">
         <v>2490</v>
       </c>
       <c r="B49" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C49" s="11"/>
-    </row>
-    <row r="50" spans="1:3">
+      <c r="D49" s="11"/>
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50" s="8" t="s">
         <v>2491</v>
       </c>
       <c r="B50" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C50" s="11"/>
-    </row>
-    <row r="51" spans="1:3">
+      <c r="D50" s="11"/>
+    </row>
+    <row r="51" spans="1:4">
       <c r="A51" s="8" t="s">
         <v>2492</v>
       </c>
       <c r="B51" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C51" s="11"/>
-    </row>
-    <row r="52" spans="1:3">
+      <c r="D51" s="11"/>
+    </row>
+    <row r="52" spans="1:4">
       <c r="A52" s="8" t="s">
         <v>2493</v>
       </c>
       <c r="B52" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C52" s="11"/>
-    </row>
-    <row r="53" spans="1:3">
+      <c r="D52" s="11"/>
+    </row>
+    <row r="53" spans="1:4">
       <c r="A53" s="8" t="s">
         <v>2494</v>
       </c>
       <c r="B53" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C53" s="11"/>
-    </row>
-    <row r="54" spans="1:3">
+      <c r="D53" s="11"/>
+    </row>
+    <row r="54" spans="1:4">
       <c r="A54" s="8" t="s">
         <v>2495</v>
       </c>
       <c r="B54" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C54" s="11"/>
-    </row>
-    <row r="55" spans="1:3">
+      <c r="D54" s="11"/>
+    </row>
+    <row r="55" spans="1:4">
       <c r="A55" s="8" t="s">
         <v>2496</v>
       </c>
       <c r="B55" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C55" s="11"/>
-    </row>
-    <row r="56" spans="1:3">
+      <c r="D55" s="11"/>
+    </row>
+    <row r="56" spans="1:4">
       <c r="A56" s="8" t="s">
         <v>2497</v>
       </c>
       <c r="B56" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C56" s="11"/>
-    </row>
-    <row r="57" spans="1:3">
+      <c r="D56" s="11"/>
+    </row>
+    <row r="57" spans="1:4">
       <c r="A57" s="8" t="s">
         <v>2498</v>
       </c>
       <c r="B57" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C57" s="11"/>
-    </row>
-    <row r="58" spans="1:3">
+      <c r="D57" s="11"/>
+    </row>
+    <row r="58" spans="1:4">
       <c r="A58" s="8" t="s">
         <v>2499</v>
       </c>
       <c r="B58" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C58" s="11"/>
-    </row>
-    <row r="59" spans="1:3">
+      <c r="D58" s="11"/>
+    </row>
+    <row r="59" spans="1:4">
       <c r="A59" s="8" t="s">
         <v>2500</v>
       </c>
       <c r="B59" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C59" s="11"/>
-    </row>
-    <row r="60" spans="1:3">
+      <c r="D59" s="11"/>
+    </row>
+    <row r="60" spans="1:4">
       <c r="A60" s="8" t="s">
         <v>2501</v>
       </c>
       <c r="B60" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C60" s="11"/>
-    </row>
-    <row r="61" spans="1:3">
+      <c r="D60" s="11"/>
+    </row>
+    <row r="61" spans="1:4">
       <c r="A61" s="8" t="s">
         <v>2502</v>
       </c>
       <c r="B61" s="7" t="s">
         <v>2625</v>
       </c>
-      <c r="C61" s="11"/>
-    </row>
-    <row r="62" spans="1:3">
+      <c r="D61" s="11"/>
+    </row>
+    <row r="62" spans="1:4">
       <c r="A62" s="8" t="s">
         <v>2503</v>
       </c>
       <c r="B62" s="7" t="s">
         <v>2625</v>
       </c>
-      <c r="C62" s="11"/>
-    </row>
-    <row r="63" spans="1:3">
+      <c r="D62" s="11"/>
+    </row>
+    <row r="63" spans="1:4">
       <c r="A63" s="8" t="s">
         <v>2504</v>
       </c>
       <c r="B63" s="7" t="s">
         <v>2625</v>
       </c>
-      <c r="C63" s="11"/>
-    </row>
-    <row r="64" spans="1:3">
+      <c r="D63" s="11"/>
+    </row>
+    <row r="64" spans="1:4">
       <c r="A64" s="8" t="s">
         <v>2505</v>
       </c>
       <c r="B64" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C64" s="11"/>
-    </row>
-    <row r="65" spans="1:3">
+      <c r="D64" s="11"/>
+    </row>
+    <row r="65" spans="1:4">
       <c r="A65" s="8" t="s">
         <v>2506</v>
       </c>
       <c r="B65" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C65" s="11"/>
-    </row>
-    <row r="66" spans="1:3">
+      <c r="D65" s="11"/>
+    </row>
+    <row r="66" spans="1:4">
       <c r="A66" s="8" t="s">
         <v>2507</v>
       </c>
       <c r="B66" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C66" s="11"/>
-    </row>
-    <row r="67" spans="1:3">
+      <c r="D66" s="11"/>
+    </row>
+    <row r="67" spans="1:4">
       <c r="A67" s="8" t="s">
         <v>2508</v>
       </c>
       <c r="B67" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C67" s="11"/>
-    </row>
-    <row r="68" spans="1:3">
+      <c r="D67" s="11"/>
+    </row>
+    <row r="68" spans="1:4">
       <c r="A68" s="8" t="s">
         <v>2509</v>
       </c>
       <c r="B68" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C68" s="11"/>
-    </row>
-    <row r="69" spans="1:3">
+      <c r="D68" s="11"/>
+    </row>
+    <row r="69" spans="1:4">
       <c r="A69" s="8" t="s">
         <v>2510</v>
       </c>
       <c r="B69" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C69" s="11"/>
-    </row>
-    <row r="70" spans="1:3">
+      <c r="D69" s="11"/>
+    </row>
+    <row r="70" spans="1:4">
       <c r="A70" s="8" t="s">
         <v>2511</v>
       </c>
       <c r="B70" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C70" s="11"/>
-    </row>
-    <row r="71" spans="1:3">
+      <c r="D70" s="11"/>
+    </row>
+    <row r="71" spans="1:4">
       <c r="A71" s="8" t="s">
         <v>2512</v>
       </c>
       <c r="B71" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C71" s="11"/>
-    </row>
-    <row r="72" spans="1:3">
+      <c r="D71" s="11"/>
+    </row>
+    <row r="72" spans="1:4">
       <c r="A72" s="8" t="s">
         <v>2513</v>
       </c>
       <c r="B72" s="7" t="s">
         <v>2625</v>
       </c>
-      <c r="C72" s="11"/>
-    </row>
-    <row r="73" spans="1:3">
+      <c r="D72" s="11"/>
+    </row>
+    <row r="73" spans="1:4">
       <c r="A73" s="8" t="s">
         <v>2514</v>
       </c>
       <c r="B73" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C73" s="11"/>
-    </row>
-    <row r="74" spans="1:3">
+      <c r="D73" s="11"/>
+    </row>
+    <row r="74" spans="1:4">
       <c r="A74" s="8" t="s">
         <v>2515</v>
       </c>
       <c r="B74" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C74" s="11"/>
-    </row>
-    <row r="75" spans="1:3">
+      <c r="D74" s="11"/>
+    </row>
+    <row r="75" spans="1:4">
       <c r="A75" s="8" t="s">
         <v>2516</v>
       </c>
       <c r="B75" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C75" s="11"/>
-    </row>
-    <row r="76" spans="1:3">
+      <c r="D75" s="11"/>
+    </row>
+    <row r="76" spans="1:4">
       <c r="A76" s="8" t="s">
         <v>2517</v>
       </c>
       <c r="B76" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C76" s="11"/>
-    </row>
-    <row r="77" spans="1:3">
+      <c r="D76" s="11"/>
+    </row>
+    <row r="77" spans="1:4">
       <c r="A77" s="8" t="s">
         <v>2518</v>
       </c>
       <c r="B77" s="7" t="s">
         <v>2625</v>
       </c>
-      <c r="C77" s="11"/>
-    </row>
-    <row r="78" spans="1:3">
+      <c r="D77" s="11"/>
+    </row>
+    <row r="78" spans="1:4">
       <c r="A78" s="8" t="s">
         <v>2519</v>
       </c>
       <c r="B78" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C78" s="11"/>
-    </row>
-    <row r="79" spans="1:3">
+      <c r="D78" s="11"/>
+    </row>
+    <row r="79" spans="1:4">
       <c r="A79" s="8" t="s">
         <v>2520</v>
       </c>
       <c r="B79" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C79" s="11"/>
-    </row>
-    <row r="80" spans="1:3">
+      <c r="D79" s="11"/>
+    </row>
+    <row r="80" spans="1:4">
       <c r="A80" s="8" t="s">
         <v>2521</v>
       </c>
       <c r="B80" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C80" s="11"/>
-    </row>
-    <row r="81" spans="1:3">
+      <c r="D80" s="11"/>
+    </row>
+    <row r="81" spans="1:4">
       <c r="A81" s="8" t="s">
         <v>2522</v>
       </c>
       <c r="B81" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C81" s="11"/>
-    </row>
-    <row r="82" spans="1:3">
+      <c r="D81" s="11"/>
+    </row>
+    <row r="82" spans="1:4">
       <c r="A82" s="8" t="s">
         <v>2523</v>
       </c>
       <c r="B82" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C82" s="11"/>
-    </row>
-    <row r="83" spans="1:3">
+      <c r="D82" s="11"/>
+    </row>
+    <row r="83" spans="1:4">
       <c r="A83" s="8" t="s">
         <v>2524</v>
       </c>
       <c r="B83" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C83" s="11"/>
-    </row>
-    <row r="84" spans="1:3">
+      <c r="D83" s="11"/>
+    </row>
+    <row r="84" spans="1:4">
       <c r="A84" s="8" t="s">
         <v>2525</v>
       </c>
       <c r="B84" s="7" t="s">
         <v>2625</v>
       </c>
-      <c r="C84" s="11"/>
-    </row>
-    <row r="85" spans="1:3">
+      <c r="D84" s="11"/>
+    </row>
+    <row r="85" spans="1:4">
       <c r="A85" s="8" t="s">
         <v>2526</v>
       </c>
       <c r="B85" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C85" s="11"/>
-    </row>
-    <row r="86" spans="1:3">
+      <c r="D85" s="11"/>
+    </row>
+    <row r="86" spans="1:4">
       <c r="A86" s="8" t="s">
         <v>2527</v>
       </c>
       <c r="B86" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C86" s="11"/>
-    </row>
-    <row r="87" spans="1:3">
+      <c r="D86" s="11"/>
+    </row>
+    <row r="87" spans="1:4">
       <c r="A87" s="8" t="s">
         <v>2528</v>
       </c>
       <c r="B87" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C87" s="11"/>
-    </row>
-    <row r="88" spans="1:3">
+      <c r="D87" s="11"/>
+    </row>
+    <row r="88" spans="1:4">
       <c r="A88" s="8" t="s">
         <v>2529</v>
       </c>
       <c r="B88" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C88" s="11"/>
-    </row>
-    <row r="89" spans="1:3">
+      <c r="D88" s="11"/>
+    </row>
+    <row r="89" spans="1:4">
       <c r="A89" s="8" t="s">
         <v>2530</v>
       </c>
       <c r="B89" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C89" s="11"/>
-    </row>
-    <row r="90" spans="1:3">
+      <c r="D89" s="11"/>
+    </row>
+    <row r="90" spans="1:4">
       <c r="A90" s="8" t="s">
         <v>2531</v>
       </c>
       <c r="B90" s="7" t="s">
         <v>2625</v>
       </c>
-      <c r="C90" s="11"/>
-    </row>
-    <row r="91" spans="1:3">
+      <c r="D90" s="11"/>
+    </row>
+    <row r="91" spans="1:4">
       <c r="A91" s="8" t="s">
         <v>2532</v>
       </c>
       <c r="B91" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C91" s="11"/>
-    </row>
-    <row r="92" spans="1:3">
+      <c r="D91" s="11"/>
+    </row>
+    <row r="92" spans="1:4">
       <c r="A92" s="8" t="s">
         <v>2533</v>
       </c>
       <c r="B92" s="7" t="s">
         <v>2625</v>
       </c>
-      <c r="C92" s="11"/>
-    </row>
-    <row r="93" spans="1:3">
+      <c r="D92" s="11"/>
+    </row>
+    <row r="93" spans="1:4">
       <c r="A93" s="8" t="s">
         <v>2534</v>
       </c>
       <c r="B93" s="7" t="s">
         <v>2625</v>
       </c>
-      <c r="C93" s="11"/>
-    </row>
-    <row r="94" spans="1:3">
+      <c r="D93" s="11"/>
+    </row>
+    <row r="94" spans="1:4">
       <c r="A94" s="8" t="s">
         <v>2535</v>
       </c>
       <c r="B94" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C94" s="11"/>
-    </row>
-    <row r="95" spans="1:3">
+      <c r="D94" s="11"/>
+    </row>
+    <row r="95" spans="1:4">
       <c r="A95" s="8" t="s">
         <v>2536</v>
       </c>
       <c r="B95" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C95" s="11"/>
-    </row>
-    <row r="96" spans="1:3">
+      <c r="D95" s="11"/>
+    </row>
+    <row r="96" spans="1:4">
       <c r="A96" s="8" t="s">
         <v>2537</v>
       </c>
       <c r="B96" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C96" s="11"/>
-    </row>
-    <row r="97" spans="1:3">
+      <c r="D96" s="11"/>
+    </row>
+    <row r="97" spans="1:4">
       <c r="A97" s="8" t="s">
         <v>2538</v>
       </c>
       <c r="B97" s="7" t="s">
         <v>2625</v>
       </c>
-      <c r="C97" s="11"/>
-    </row>
-    <row r="98" spans="1:3">
+      <c r="D97" s="11"/>
+    </row>
+    <row r="98" spans="1:4">
       <c r="A98" s="8" t="s">
         <v>2539</v>
       </c>
       <c r="B98" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C98" s="11"/>
-    </row>
-    <row r="99" spans="1:3">
+      <c r="D98" s="11"/>
+    </row>
+    <row r="99" spans="1:4">
       <c r="A99" s="8" t="s">
         <v>2540</v>
       </c>
       <c r="B99" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C99" s="11"/>
-    </row>
-    <row r="100" spans="1:3">
+      <c r="D99" s="11"/>
+    </row>
+    <row r="100" spans="1:4">
       <c r="A100" s="8" t="s">
         <v>2541</v>
       </c>
       <c r="B100" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C100" s="11"/>
-    </row>
-    <row r="101" spans="1:3">
+      <c r="D100" s="11"/>
+    </row>
+    <row r="101" spans="1:4">
       <c r="A101" s="8" t="s">
         <v>2542</v>
       </c>
       <c r="B101" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C101" s="11"/>
-    </row>
-    <row r="102" spans="1:3">
+      <c r="D101" s="11"/>
+    </row>
+    <row r="102" spans="1:4">
       <c r="A102" s="8" t="s">
         <v>2543</v>
       </c>
       <c r="B102" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C102" s="11"/>
-    </row>
-    <row r="103" spans="1:3">
+      <c r="D102" s="11"/>
+    </row>
+    <row r="103" spans="1:4">
       <c r="A103" s="8" t="s">
         <v>2544</v>
       </c>
       <c r="B103" s="7" t="s">
         <v>2625</v>
       </c>
-      <c r="C103" s="11"/>
-    </row>
-    <row r="104" spans="1:3">
+      <c r="D103" s="11"/>
+    </row>
+    <row r="104" spans="1:4">
       <c r="A104" s="8" t="s">
         <v>2545</v>
       </c>
       <c r="B104" s="7" t="s">
         <v>2625</v>
       </c>
-      <c r="C104" s="11"/>
-    </row>
-    <row r="105" spans="1:3">
+      <c r="D104" s="11"/>
+    </row>
+    <row r="105" spans="1:4">
       <c r="A105" s="8" t="s">
         <v>2546</v>
       </c>
       <c r="B105" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C105" s="11"/>
-    </row>
-    <row r="106" spans="1:3">
+      <c r="D105" s="11"/>
+    </row>
+    <row r="106" spans="1:4">
       <c r="A106" s="8" t="s">
         <v>2547</v>
       </c>
       <c r="B106" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C106" s="11"/>
-    </row>
-    <row r="107" spans="1:3">
+      <c r="D106" s="11"/>
+    </row>
+    <row r="107" spans="1:4">
       <c r="A107" s="8" t="s">
         <v>2548</v>
       </c>
       <c r="B107" s="7" t="s">
         <v>2625</v>
       </c>
-      <c r="C107" s="11"/>
-    </row>
-    <row r="108" spans="1:3">
+      <c r="D107" s="11"/>
+    </row>
+    <row r="108" spans="1:4">
       <c r="A108" s="8" t="s">
         <v>2549</v>
       </c>
       <c r="B108" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C108" s="11"/>
-    </row>
-    <row r="109" spans="1:3">
+      <c r="D108" s="11"/>
+    </row>
+    <row r="109" spans="1:4">
       <c r="A109" s="8" t="s">
         <v>1356</v>
       </c>
       <c r="B109" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C109" s="11"/>
-    </row>
-    <row r="110" spans="1:3">
+      <c r="D109" s="11"/>
+    </row>
+    <row r="110" spans="1:4">
       <c r="A110" s="8" t="s">
         <v>2550</v>
       </c>
       <c r="B110" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C110" s="11" t="s">
+      <c r="D110" s="11" t="s">
         <v>3390</v>
       </c>
     </row>
-    <row r="111" spans="1:3">
+    <row r="111" spans="1:4">
       <c r="A111" s="8" t="s">
         <v>2551</v>
       </c>
       <c r="B111" s="7" t="s">
         <v>2625</v>
       </c>
-      <c r="C111" s="11"/>
-    </row>
-    <row r="112" spans="1:3">
+      <c r="D111" s="11"/>
+    </row>
+    <row r="112" spans="1:4">
       <c r="A112" s="8" t="s">
         <v>2552</v>
       </c>
       <c r="B112" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C112" s="11"/>
-    </row>
-    <row r="113" spans="1:3">
+      <c r="D112" s="11"/>
+    </row>
+    <row r="113" spans="1:4">
       <c r="A113" s="8" t="s">
         <v>2553</v>
       </c>
       <c r="B113" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C113" s="11"/>
-    </row>
-    <row r="114" spans="1:3">
+      <c r="D113" s="11"/>
+    </row>
+    <row r="114" spans="1:4">
       <c r="A114" s="8" t="s">
         <v>2554</v>
       </c>
       <c r="B114" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C114" s="11"/>
-    </row>
-    <row r="115" spans="1:3">
+      <c r="D114" s="11"/>
+    </row>
+    <row r="115" spans="1:4">
       <c r="A115" s="8" t="s">
         <v>2555</v>
       </c>
       <c r="B115" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C115" s="11"/>
-    </row>
-    <row r="116" spans="1:3">
+      <c r="D115" s="11"/>
+    </row>
+    <row r="116" spans="1:4">
       <c r="A116" s="8" t="s">
         <v>2556</v>
       </c>
       <c r="B116" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C116" s="11"/>
-    </row>
-    <row r="117" spans="1:3">
+      <c r="D116" s="11"/>
+    </row>
+    <row r="117" spans="1:4">
       <c r="A117" s="8" t="s">
         <v>2557</v>
       </c>
       <c r="B117" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C117" s="11"/>
-    </row>
-    <row r="118" spans="1:3">
+      <c r="D117" s="11"/>
+    </row>
+    <row r="118" spans="1:4">
       <c r="A118" s="8" t="s">
         <v>2558</v>
       </c>
       <c r="B118" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C118" s="11"/>
-    </row>
-    <row r="119" spans="1:3">
+      <c r="D118" s="11"/>
+    </row>
+    <row r="119" spans="1:4">
       <c r="A119" s="8" t="s">
         <v>2559</v>
       </c>
       <c r="B119" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C119" s="11"/>
-    </row>
-    <row r="120" spans="1:3">
+      <c r="D119" s="11"/>
+    </row>
+    <row r="120" spans="1:4">
       <c r="A120" s="8" t="s">
         <v>2560</v>
       </c>
       <c r="B120" s="7" t="s">
         <v>2625</v>
       </c>
-      <c r="C120" s="11"/>
-    </row>
-    <row r="121" spans="1:3">
+      <c r="D120" s="11"/>
+    </row>
+    <row r="121" spans="1:4">
       <c r="A121" s="8" t="s">
         <v>2561</v>
       </c>
       <c r="B121" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C121" s="11"/>
-    </row>
-    <row r="122" spans="1:3">
+      <c r="D121" s="11"/>
+    </row>
+    <row r="122" spans="1:4">
       <c r="A122" s="8" t="s">
         <v>2562</v>
       </c>
       <c r="B122" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C122" s="11"/>
-    </row>
-    <row r="123" spans="1:3">
+      <c r="D122" s="11"/>
+    </row>
+    <row r="123" spans="1:4">
       <c r="A123" s="8" t="s">
         <v>2563</v>
       </c>
       <c r="B123" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C123" s="11"/>
-    </row>
-    <row r="124" spans="1:3">
+      <c r="D123" s="11"/>
+    </row>
+    <row r="124" spans="1:4">
       <c r="A124" s="8" t="s">
         <v>2564</v>
       </c>
       <c r="B124" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C124" s="11"/>
-    </row>
-    <row r="125" spans="1:3">
+      <c r="D124" s="11"/>
+    </row>
+    <row r="125" spans="1:4">
       <c r="A125" s="8" t="s">
         <v>2565</v>
       </c>
       <c r="B125" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C125" s="11"/>
-    </row>
-    <row r="126" spans="1:3">
+      <c r="D125" s="11"/>
+    </row>
+    <row r="126" spans="1:4">
       <c r="A126" s="8" t="s">
         <v>2566</v>
       </c>
       <c r="B126" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C126" s="11"/>
-    </row>
-    <row r="127" spans="1:3">
+      <c r="D126" s="11"/>
+    </row>
+    <row r="127" spans="1:4">
       <c r="A127" s="8" t="s">
         <v>2567</v>
       </c>
       <c r="B127" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C127" s="11"/>
-    </row>
-    <row r="128" spans="1:3">
+      <c r="D127" s="11"/>
+    </row>
+    <row r="128" spans="1:4">
       <c r="A128" s="8" t="s">
         <v>2568</v>
       </c>
       <c r="B128" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C128" s="11"/>
-    </row>
-    <row r="129" spans="1:3">
+      <c r="D128" s="11"/>
+    </row>
+    <row r="129" spans="1:4">
       <c r="A129" s="8" t="s">
         <v>2569</v>
       </c>
       <c r="B129" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C129" s="11"/>
-    </row>
-    <row r="130" spans="1:3">
+      <c r="D129" s="11"/>
+    </row>
+    <row r="130" spans="1:4">
       <c r="A130" s="8" t="s">
         <v>2570</v>
       </c>
       <c r="B130" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C130" s="11"/>
-    </row>
-    <row r="131" spans="1:3">
+      <c r="D130" s="11"/>
+    </row>
+    <row r="131" spans="1:4">
       <c r="A131" s="8" t="s">
         <v>2571</v>
       </c>
       <c r="B131" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C131" s="11"/>
-    </row>
-    <row r="132" spans="1:3">
+      <c r="D131" s="11"/>
+    </row>
+    <row r="132" spans="1:4">
       <c r="A132" s="8" t="s">
         <v>2572</v>
       </c>
       <c r="B132" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C132" s="11"/>
-    </row>
-    <row r="133" spans="1:3">
+      <c r="D132" s="11"/>
+    </row>
+    <row r="133" spans="1:4">
       <c r="A133" s="8" t="s">
         <v>2573</v>
       </c>
       <c r="B133" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C133" s="11"/>
-    </row>
-    <row r="134" spans="1:3">
+      <c r="D133" s="11"/>
+    </row>
+    <row r="134" spans="1:4">
       <c r="A134" s="8" t="s">
         <v>2574</v>
       </c>
       <c r="B134" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C134" s="11"/>
-    </row>
-    <row r="135" spans="1:3">
+      <c r="D134" s="11"/>
+    </row>
+    <row r="135" spans="1:4">
       <c r="A135" s="8" t="s">
         <v>2575</v>
       </c>
       <c r="B135" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C135" s="11"/>
-    </row>
-    <row r="136" spans="1:3">
+      <c r="D135" s="11"/>
+    </row>
+    <row r="136" spans="1:4">
       <c r="A136" s="8" t="s">
         <v>2576</v>
       </c>
       <c r="B136" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C136" s="11"/>
-    </row>
-    <row r="137" spans="1:3">
+      <c r="D136" s="11"/>
+    </row>
+    <row r="137" spans="1:4">
       <c r="A137" s="8" t="s">
         <v>2577</v>
       </c>
       <c r="B137" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C137" s="11"/>
-    </row>
-    <row r="138" spans="1:3">
+      <c r="D137" s="11"/>
+    </row>
+    <row r="138" spans="1:4">
       <c r="A138" s="8" t="s">
         <v>2578</v>
       </c>
       <c r="B138" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C138" s="11"/>
-    </row>
-    <row r="139" spans="1:3">
+      <c r="D138" s="11"/>
+    </row>
+    <row r="139" spans="1:4">
       <c r="A139" s="8" t="s">
         <v>2579</v>
       </c>
       <c r="B139" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C139" s="11"/>
-    </row>
-    <row r="140" spans="1:3">
+      <c r="D139" s="11"/>
+    </row>
+    <row r="140" spans="1:4">
       <c r="A140" s="8" t="s">
         <v>2580</v>
       </c>
       <c r="B140" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C140" s="11"/>
-    </row>
-    <row r="141" spans="1:3">
+      <c r="D140" s="11"/>
+    </row>
+    <row r="141" spans="1:4">
       <c r="A141" s="8" t="s">
         <v>2581</v>
       </c>
       <c r="B141" s="7" t="s">
         <v>2625</v>
       </c>
-      <c r="C141" s="11"/>
-    </row>
-    <row r="142" spans="1:3">
+      <c r="D141" s="11"/>
+    </row>
+    <row r="142" spans="1:4">
       <c r="A142" s="8" t="s">
         <v>2582</v>
       </c>
       <c r="B142" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C142" s="11"/>
-    </row>
-    <row r="143" spans="1:3">
+      <c r="D142" s="11"/>
+    </row>
+    <row r="143" spans="1:4">
       <c r="A143" s="8" t="s">
         <v>2583</v>
       </c>
       <c r="B143" s="7" t="s">
         <v>2625</v>
       </c>
-      <c r="C143" s="11"/>
-    </row>
-    <row r="144" spans="1:3">
+      <c r="D143" s="11"/>
+    </row>
+    <row r="144" spans="1:4">
       <c r="A144" s="8" t="s">
         <v>2584</v>
       </c>
       <c r="B144" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C144" s="11"/>
-    </row>
-    <row r="145" spans="1:3">
+      <c r="D144" s="11"/>
+    </row>
+    <row r="145" spans="1:4">
       <c r="A145" s="8" t="s">
         <v>2585</v>
       </c>
       <c r="B145" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C145" s="11"/>
-    </row>
-    <row r="146" spans="1:3">
+      <c r="D145" s="11"/>
+    </row>
+    <row r="146" spans="1:4">
       <c r="A146" s="8" t="s">
         <v>2586</v>
       </c>
       <c r="B146" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C146" s="11"/>
-    </row>
-    <row r="147" spans="1:3">
+      <c r="D146" s="11"/>
+    </row>
+    <row r="147" spans="1:4">
       <c r="A147" s="8" t="s">
         <v>2587</v>
       </c>
       <c r="B147" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C147" s="11"/>
-    </row>
-    <row r="148" spans="1:3">
+      <c r="D147" s="11"/>
+    </row>
+    <row r="148" spans="1:4">
       <c r="A148" s="8" t="s">
         <v>2588</v>
       </c>
       <c r="B148" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C148" s="11"/>
-    </row>
-    <row r="149" spans="1:3">
+      <c r="D148" s="11"/>
+    </row>
+    <row r="149" spans="1:4">
       <c r="A149" s="8" t="s">
         <v>2589</v>
       </c>
       <c r="B149" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C149" s="11"/>
-    </row>
-    <row r="150" spans="1:3">
+      <c r="D149" s="11"/>
+    </row>
+    <row r="150" spans="1:4">
       <c r="A150" s="8" t="s">
         <v>2590</v>
       </c>
       <c r="B150" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C150" s="11"/>
-    </row>
-    <row r="151" spans="1:3">
+      <c r="D150" s="11"/>
+    </row>
+    <row r="151" spans="1:4">
       <c r="A151" s="8" t="s">
         <v>2591</v>
       </c>
       <c r="B151" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C151" s="11"/>
-    </row>
-    <row r="152" spans="1:3">
+      <c r="D151" s="11"/>
+    </row>
+    <row r="152" spans="1:4">
       <c r="A152" s="8" t="s">
         <v>2592</v>
       </c>
       <c r="B152" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C152" s="11"/>
-    </row>
-    <row r="153" spans="1:3">
+      <c r="D152" s="11"/>
+    </row>
+    <row r="153" spans="1:4">
       <c r="A153" s="8" t="s">
         <v>2593</v>
       </c>
       <c r="B153" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C153" s="11"/>
-    </row>
-    <row r="154" spans="1:3">
+      <c r="D153" s="11"/>
+    </row>
+    <row r="154" spans="1:4">
       <c r="A154" s="8" t="s">
         <v>2594</v>
       </c>
       <c r="B154" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C154" s="11"/>
-    </row>
-    <row r="155" spans="1:3">
+      <c r="D154" s="11"/>
+    </row>
+    <row r="155" spans="1:4">
       <c r="A155" s="8" t="s">
         <v>2595</v>
       </c>
       <c r="B155" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C155" s="11"/>
-    </row>
-    <row r="156" spans="1:3">
+      <c r="D155" s="11"/>
+    </row>
+    <row r="156" spans="1:4">
       <c r="A156" s="8" t="s">
         <v>2596</v>
       </c>
       <c r="B156" s="7" t="s">
         <v>2625</v>
       </c>
-      <c r="C156" s="11"/>
-    </row>
-    <row r="157" spans="1:3">
+      <c r="D156" s="11"/>
+    </row>
+    <row r="157" spans="1:4">
       <c r="A157" s="8" t="s">
         <v>2597</v>
       </c>
       <c r="B157" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C157" s="11"/>
-    </row>
-    <row r="158" spans="1:3">
+      <c r="D157" s="11"/>
+    </row>
+    <row r="158" spans="1:4">
       <c r="A158" s="8" t="s">
         <v>2598</v>
       </c>
       <c r="B158" s="7" t="s">
         <v>2625</v>
       </c>
-      <c r="C158" s="11"/>
-    </row>
-    <row r="159" spans="1:3">
+      <c r="D158" s="11"/>
+    </row>
+    <row r="159" spans="1:4">
       <c r="A159" s="8" t="s">
         <v>2599</v>
       </c>
       <c r="B159" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C159" s="11"/>
-    </row>
-    <row r="160" spans="1:3">
+      <c r="D159" s="11"/>
+    </row>
+    <row r="160" spans="1:4">
       <c r="A160" s="8" t="s">
         <v>2600</v>
       </c>
       <c r="B160" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C160" s="11"/>
-    </row>
-    <row r="161" spans="1:3">
+      <c r="D160" s="11"/>
+    </row>
+    <row r="161" spans="1:4">
       <c r="A161" s="8" t="s">
         <v>2624</v>
       </c>
       <c r="B161" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C161" s="11"/>
-    </row>
-    <row r="162" spans="1:3">
+      <c r="D161" s="11"/>
+    </row>
+    <row r="162" spans="1:4">
       <c r="A162" s="8" t="s">
         <v>2601</v>
       </c>
       <c r="B162" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C162" s="11"/>
-    </row>
-    <row r="163" spans="1:3">
+      <c r="D162" s="11"/>
+    </row>
+    <row r="163" spans="1:4">
       <c r="A163" s="8" t="s">
         <v>2602</v>
       </c>
       <c r="B163" s="7" t="s">
         <v>2625</v>
       </c>
-      <c r="C163" s="11"/>
-    </row>
-    <row r="164" spans="1:3">
+      <c r="D163" s="11"/>
+    </row>
+    <row r="164" spans="1:4">
       <c r="A164" s="8" t="s">
         <v>2603</v>
       </c>
       <c r="B164" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C164" s="11"/>
-    </row>
-    <row r="165" spans="1:3">
+      <c r="D164" s="11"/>
+    </row>
+    <row r="165" spans="1:4">
       <c r="A165" s="8" t="s">
         <v>2604</v>
       </c>
       <c r="B165" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C165" s="11"/>
-    </row>
-    <row r="166" spans="1:3">
+      <c r="D165" s="11"/>
+    </row>
+    <row r="166" spans="1:4">
       <c r="A166" s="8" t="s">
         <v>2605</v>
       </c>
       <c r="B166" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C166" s="11"/>
-    </row>
-    <row r="167" spans="1:3">
+      <c r="D166" s="11"/>
+    </row>
+    <row r="167" spans="1:4">
       <c r="A167" s="8" t="s">
         <v>2606</v>
       </c>
       <c r="B167" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C167" s="11"/>
-    </row>
-    <row r="168" spans="1:3">
+      <c r="D167" s="11"/>
+    </row>
+    <row r="168" spans="1:4">
       <c r="A168" s="8" t="s">
         <v>2607</v>
       </c>
       <c r="B168" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C168" s="11"/>
-    </row>
-    <row r="169" spans="1:3">
+      <c r="D168" s="11"/>
+    </row>
+    <row r="169" spans="1:4">
       <c r="A169" s="8" t="s">
         <v>2608</v>
       </c>
       <c r="B169" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C169" s="11"/>
-    </row>
-    <row r="170" spans="1:3">
+      <c r="D169" s="11"/>
+    </row>
+    <row r="170" spans="1:4">
       <c r="A170" s="8" t="s">
         <v>2609</v>
       </c>
       <c r="B170" s="7" t="s">
         <v>2625</v>
       </c>
-      <c r="C170" s="11"/>
-    </row>
-    <row r="171" spans="1:3">
+      <c r="D170" s="11"/>
+    </row>
+    <row r="171" spans="1:4">
       <c r="A171" s="8" t="s">
         <v>2610</v>
       </c>
       <c r="B171" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C171" s="11"/>
-    </row>
-    <row r="172" spans="1:3">
+      <c r="D171" s="11"/>
+    </row>
+    <row r="172" spans="1:4">
       <c r="A172" s="8" t="s">
         <v>2611</v>
       </c>
       <c r="B172" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C172" s="11"/>
-    </row>
-    <row r="173" spans="1:3">
+      <c r="D172" s="11"/>
+    </row>
+    <row r="173" spans="1:4">
       <c r="A173" s="8" t="s">
         <v>2612</v>
       </c>
       <c r="B173" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C173" s="11"/>
-    </row>
-    <row r="174" spans="1:3">
+      <c r="D173" s="11"/>
+    </row>
+    <row r="174" spans="1:4">
       <c r="A174" s="8" t="s">
         <v>2613</v>
       </c>
       <c r="B174" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C174" s="11"/>
-    </row>
-    <row r="175" spans="1:3">
+      <c r="D174" s="11"/>
+    </row>
+    <row r="175" spans="1:4">
       <c r="A175" s="8" t="s">
         <v>2614</v>
       </c>
       <c r="B175" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C175" s="11"/>
-    </row>
-    <row r="176" spans="1:3">
+      <c r="D175" s="11"/>
+    </row>
+    <row r="176" spans="1:4">
       <c r="A176" s="8" t="s">
         <v>2615</v>
       </c>
       <c r="B176" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C176" s="11"/>
-    </row>
-    <row r="177" spans="1:3">
+      <c r="D176" s="11"/>
+    </row>
+    <row r="177" spans="1:4">
       <c r="A177" s="8" t="s">
         <v>2616</v>
       </c>
       <c r="B177" s="7" t="s">
         <v>2625</v>
       </c>
-      <c r="C177" s="11"/>
-    </row>
-    <row r="178" spans="1:3">
+      <c r="D177" s="11"/>
+    </row>
+    <row r="178" spans="1:4">
       <c r="A178" s="8" t="s">
         <v>2617</v>
       </c>
       <c r="B178" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C178" s="11"/>
-    </row>
-    <row r="179" spans="1:3">
+      <c r="D178" s="11"/>
+    </row>
+    <row r="179" spans="1:4">
       <c r="A179" s="8" t="s">
         <v>2618</v>
       </c>
       <c r="B179" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C179" s="11"/>
-    </row>
-    <row r="180" spans="1:3">
+      <c r="D179" s="11"/>
+    </row>
+    <row r="180" spans="1:4">
       <c r="A180" s="8" t="s">
         <v>2619</v>
       </c>
       <c r="B180" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C180" s="11"/>
-    </row>
-    <row r="181" spans="1:3">
+      <c r="D180" s="11"/>
+    </row>
+    <row r="181" spans="1:4">
       <c r="A181" s="8" t="s">
         <v>2620</v>
       </c>
       <c r="B181" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C181" s="11"/>
-    </row>
-    <row r="182" spans="1:3">
+      <c r="D181" s="11"/>
+    </row>
+    <row r="182" spans="1:4">
       <c r="A182" s="8" t="s">
         <v>2621</v>
       </c>
       <c r="B182" s="7" t="s">
         <v>2247</v>
       </c>
-      <c r="C182" s="11"/>
-    </row>
-    <row r="183" spans="1:3">
+      <c r="D182" s="11"/>
+    </row>
+    <row r="183" spans="1:4">
       <c r="A183" s="8" t="s">
         <v>2622</v>
       </c>
       <c r="B183" s="7" t="s">
         <v>2625</v>
       </c>
-      <c r="C183" s="11"/>
+      <c r="D183" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -12915,8 +12993,8 @@
   <dimension ref="A1:G1404"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A1129" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1126" sqref="C1126"/>
+      <pane ySplit="6" topLeftCell="A151" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C155" sqref="C155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.28515625" defaultRowHeight="11.25"/>
@@ -13293,6 +13371,9 @@
       <c r="E26" s="1" t="s">
         <v>2247</v>
       </c>
+      <c r="F26" s="1" t="s">
+        <v>3434</v>
+      </c>
       <c r="G26" s="20"/>
     </row>
     <row r="27" spans="1:7">
@@ -13311,6 +13392,9 @@
       <c r="E27" s="1" t="s">
         <v>2247</v>
       </c>
+      <c r="F27" s="1" t="s">
+        <v>3434</v>
+      </c>
       <c r="G27" s="20"/>
     </row>
     <row r="28" spans="1:7">
@@ -13670,6 +13754,9 @@
       <c r="E49" s="1" t="s">
         <v>2247</v>
       </c>
+      <c r="F49" s="1" t="s">
+        <v>3428</v>
+      </c>
       <c r="G49" s="20"/>
     </row>
     <row r="50" spans="1:7">
@@ -13802,6 +13889,9 @@
       <c r="E57" s="1" t="s">
         <v>2247</v>
       </c>
+      <c r="F57" s="1" t="s">
+        <v>3429</v>
+      </c>
       <c r="G57" s="20"/>
     </row>
     <row r="58" spans="1:7">
@@ -13946,6 +14036,9 @@
       <c r="D66" s="2" t="s">
         <v>2247</v>
       </c>
+      <c r="E66" s="1" t="s">
+        <v>2247</v>
+      </c>
       <c r="G66" s="20"/>
     </row>
     <row r="67" spans="1:7">
@@ -14471,7 +14564,9 @@
       <c r="D95" s="18" t="s">
         <v>2247</v>
       </c>
-      <c r="E95" s="19"/>
+      <c r="E95" s="19" t="s">
+        <v>2247</v>
+      </c>
       <c r="F95" s="17" t="s">
         <v>3418</v>
       </c>
@@ -14528,24 +14623,24 @@
       </c>
       <c r="G98" s="20"/>
     </row>
-    <row r="99" spans="1:7">
-      <c r="A99" s="2" t="s">
+    <row r="99" spans="1:7" ht="22.5">
+      <c r="A99" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="B99" s="2" t="s">
+      <c r="B99" s="18" t="s">
         <v>596</v>
       </c>
-      <c r="C99" s="2" t="s">
+      <c r="C99" s="18" t="s">
         <v>1502</v>
       </c>
-      <c r="D99" s="2" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E99" s="1" t="s">
-        <v>2247</v>
-      </c>
-      <c r="F99" s="1" t="s">
-        <v>3412</v>
+      <c r="D99" s="18" t="s">
+        <v>2247</v>
+      </c>
+      <c r="E99" s="19" t="s">
+        <v>2247</v>
+      </c>
+      <c r="F99" s="17" t="s">
+        <v>3427</v>
       </c>
       <c r="G99" s="20"/>
     </row>
@@ -14564,20 +14659,23 @@
       </c>
       <c r="G100" s="20"/>
     </row>
-    <row r="101" spans="1:7">
-      <c r="A101" s="2" t="s">
+    <row r="101" spans="1:7" s="22" customFormat="1" ht="22.5">
+      <c r="A101" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="B101" s="2" t="s">
+      <c r="B101" s="24" t="s">
         <v>627</v>
       </c>
-      <c r="C101" s="2" t="s">
+      <c r="C101" s="24" t="s">
         <v>2195</v>
       </c>
-      <c r="D101" s="2" t="s">
-        <v>2247</v>
-      </c>
-      <c r="G101" s="20"/>
+      <c r="D101" s="24" t="s">
+        <v>2247</v>
+      </c>
+      <c r="F101" s="22" t="s">
+        <v>3430</v>
+      </c>
+      <c r="G101" s="25"/>
     </row>
     <row r="102" spans="1:7">
       <c r="A102" s="2" t="s">
@@ -15110,6 +15208,9 @@
       <c r="D132" s="2" t="s">
         <v>2247</v>
       </c>
+      <c r="E132" s="1" t="s">
+        <v>2247</v>
+      </c>
       <c r="G132" s="20"/>
     </row>
     <row r="133" spans="1:7">
@@ -15140,6 +15241,12 @@
       <c r="D134" s="2" t="s">
         <v>2247</v>
       </c>
+      <c r="E134" s="1" t="s">
+        <v>2247</v>
+      </c>
+      <c r="F134" s="1" t="s">
+        <v>3431</v>
+      </c>
       <c r="G134" s="20"/>
     </row>
     <row r="135" spans="1:7">
@@ -15170,6 +15277,12 @@
       <c r="D136" s="2" t="s">
         <v>2247</v>
       </c>
+      <c r="E136" s="1" t="s">
+        <v>2247</v>
+      </c>
+      <c r="F136" s="1" t="s">
+        <v>3433</v>
+      </c>
       <c r="G136" s="20"/>
     </row>
     <row r="137" spans="1:7">
@@ -15200,6 +15313,9 @@
       <c r="D138" s="2" t="s">
         <v>2247</v>
       </c>
+      <c r="E138" s="1" t="s">
+        <v>2247</v>
+      </c>
       <c r="G138" s="20"/>
     </row>
     <row r="139" spans="1:7">
@@ -15215,6 +15331,9 @@
       <c r="D139" s="2" t="s">
         <v>2247</v>
       </c>
+      <c r="E139" s="1" t="s">
+        <v>2247</v>
+      </c>
       <c r="G139" s="20"/>
     </row>
     <row r="140" spans="1:7">
@@ -15230,6 +15349,12 @@
       <c r="D140" s="2" t="s">
         <v>2247</v>
       </c>
+      <c r="E140" s="1" t="s">
+        <v>2247</v>
+      </c>
+      <c r="F140" s="1" t="s">
+        <v>3434</v>
+      </c>
       <c r="G140" s="20"/>
     </row>
     <row r="141" spans="1:7">
@@ -15245,6 +15370,12 @@
       <c r="D141" s="2" t="s">
         <v>2247</v>
       </c>
+      <c r="E141" s="1" t="s">
+        <v>2247</v>
+      </c>
+      <c r="F141" s="1" t="s">
+        <v>3434</v>
+      </c>
       <c r="G141" s="20"/>
     </row>
     <row r="142" spans="1:7">
@@ -15275,6 +15406,9 @@
       <c r="D143" s="2" t="s">
         <v>2247</v>
       </c>
+      <c r="E143" s="1" t="s">
+        <v>2247</v>
+      </c>
       <c r="G143" s="20"/>
     </row>
     <row r="144" spans="1:7">
@@ -15290,6 +15424,9 @@
       <c r="D144" s="2" t="s">
         <v>2247</v>
       </c>
+      <c r="E144" s="1" t="s">
+        <v>2247</v>
+      </c>
       <c r="G144" s="20"/>
     </row>
     <row r="145" spans="1:7">
@@ -15305,6 +15442,9 @@
       <c r="D145" s="2" t="s">
         <v>2247</v>
       </c>
+      <c r="E145" s="1" t="s">
+        <v>2247</v>
+      </c>
       <c r="G145" s="20"/>
     </row>
     <row r="146" spans="1:7">
@@ -15320,6 +15460,12 @@
       <c r="D146" s="2" t="s">
         <v>2247</v>
       </c>
+      <c r="E146" s="1" t="s">
+        <v>2247</v>
+      </c>
+      <c r="F146" s="1" t="s">
+        <v>3434</v>
+      </c>
       <c r="G146" s="20"/>
     </row>
     <row r="147" spans="1:7">
@@ -15470,6 +15616,9 @@
       <c r="D156" s="2" t="s">
         <v>2247</v>
       </c>
+      <c r="E156" s="1" t="s">
+        <v>2247</v>
+      </c>
       <c r="G156" s="20"/>
     </row>
     <row r="157" spans="1:7">
@@ -15500,20 +15649,29 @@
       <c r="D158" s="2" t="s">
         <v>2247</v>
       </c>
+      <c r="E158" s="1" t="s">
+        <v>2247</v>
+      </c>
       <c r="G158" s="20"/>
     </row>
-    <row r="159" spans="1:7">
-      <c r="A159" s="2" t="s">
+    <row r="159" spans="1:7" ht="33.75">
+      <c r="A159" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="B159" s="2" t="s">
+      <c r="B159" s="27" t="s">
         <v>660</v>
       </c>
-      <c r="C159" s="2" t="s">
+      <c r="C159" s="27" t="s">
         <v>1536</v>
       </c>
-      <c r="D159" s="2" t="s">
-        <v>2247</v>
+      <c r="D159" s="27" t="s">
+        <v>2247</v>
+      </c>
+      <c r="E159" s="26" t="s">
+        <v>2247</v>
+      </c>
+      <c r="F159" s="17" t="s">
+        <v>3435</v>
       </c>
       <c r="G159" s="20"/>
     </row>
@@ -15530,6 +15688,7 @@
       <c r="D160" s="2" t="s">
         <v>2247</v>
       </c>
+      <c r="F160" s="17"/>
       <c r="G160" s="20"/>
     </row>
     <row r="161" spans="1:7">
@@ -16628,6 +16787,9 @@
       <c r="D232" s="2" t="s">
         <v>2247</v>
       </c>
+      <c r="E232" s="1" t="s">
+        <v>2247</v>
+      </c>
       <c r="G232" s="20"/>
     </row>
     <row r="233" spans="1:7">
@@ -16838,6 +17000,9 @@
       <c r="D246" s="2" t="s">
         <v>2247</v>
       </c>
+      <c r="E246" s="1" t="s">
+        <v>2247</v>
+      </c>
       <c r="G246" s="20"/>
     </row>
     <row r="247" spans="1:7">
@@ -17243,6 +17408,9 @@
       <c r="D273" s="2" t="s">
         <v>2247</v>
       </c>
+      <c r="E273" s="1" t="s">
+        <v>2247</v>
+      </c>
       <c r="G273" s="20"/>
     </row>
     <row r="274" spans="1:7">
@@ -18573,6 +18741,9 @@
       <c r="E359" s="1" t="s">
         <v>2247</v>
       </c>
+      <c r="F359" s="1" t="s">
+        <v>3434</v>
+      </c>
       <c r="G359" s="20"/>
     </row>
     <row r="360" spans="1:7">
@@ -30370,16 +30541,16 @@
       <c r="G1136" s="20"/>
     </row>
     <row r="1137" spans="1:7" ht="22.5">
-      <c r="A1137" s="24" t="s">
+      <c r="A1137" s="18" t="s">
         <v>418</v>
       </c>
-      <c r="B1137" s="24" t="s">
+      <c r="B1137" s="18" t="s">
         <v>1291</v>
       </c>
-      <c r="C1137" s="24" t="s">
+      <c r="C1137" s="18" t="s">
         <v>2231</v>
       </c>
-      <c r="D1137" s="24" t="s">
+      <c r="D1137" s="18" t="s">
         <v>2247</v>
       </c>
       <c r="E1137" s="19" t="s">
@@ -31123,6 +31294,9 @@
       <c r="D1186" s="2" t="s">
         <v>2247</v>
       </c>
+      <c r="E1186" s="1" t="s">
+        <v>2247</v>
+      </c>
       <c r="G1186" s="20"/>
     </row>
     <row r="1187" spans="1:7">
@@ -31858,6 +32032,9 @@
       <c r="D1235" s="2" t="s">
         <v>2247</v>
       </c>
+      <c r="E1235" s="1" t="s">
+        <v>2247</v>
+      </c>
       <c r="G1235" s="20"/>
     </row>
     <row r="1236" spans="1:7">
@@ -31873,6 +32050,9 @@
       <c r="D1236" s="2" t="s">
         <v>2247</v>
       </c>
+      <c r="E1236" s="1" t="s">
+        <v>2247</v>
+      </c>
       <c r="G1236" s="20"/>
     </row>
     <row r="1237" spans="1:7">
@@ -31888,6 +32068,9 @@
       <c r="D1237" s="2" t="s">
         <v>2247</v>
       </c>
+      <c r="E1237" s="1" t="s">
+        <v>2247</v>
+      </c>
       <c r="G1237" s="20"/>
     </row>
     <row r="1238" spans="1:7">
@@ -31918,6 +32101,9 @@
       <c r="D1239" s="2" t="s">
         <v>2247</v>
       </c>
+      <c r="E1239" s="1" t="s">
+        <v>2247</v>
+      </c>
       <c r="G1239" s="20"/>
     </row>
     <row r="1240" spans="1:7">
@@ -31931,6 +32117,9 @@
         <v>2138</v>
       </c>
       <c r="D1240" s="2" t="s">
+        <v>2247</v>
+      </c>
+      <c r="E1240" s="1" t="s">
         <v>2247</v>
       </c>
       <c r="G1240" s="20"/>

</xml_diff>

<commit_message>
Atualização Napeamento ETL - Novo Servidor
</commit_message>
<xml_diff>
--- a/Documentação/Migração Servidores/Cosmos003/Mapeamento ETL.xlsx
+++ b/Documentação/Migração Servidores/Cosmos003/Mapeamento ETL.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14448" uniqueCount="3892">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14441" uniqueCount="3897">
   <si>
     <t>Job</t>
   </si>
@@ -11699,6 +11699,21 @@
   </si>
   <si>
     <t>W:\Operacional\Colecao Elegiveis LogPeg e Retira em Loja\ods_colecao_elegiveis match.dtsx</t>
+  </si>
+  <si>
+    <t>Não existe o banco MIS_TMP no servidor</t>
+  </si>
+  <si>
+    <t>está com todos os procedimentos desabilitados</t>
+  </si>
+  <si>
+    <t>precisa colocar as siglas nas caixinhas do "(DFT) SIGE &gt; TMP"</t>
+  </si>
+  <si>
+    <t>precisa colocar as siglas nas caixinhas</t>
+  </si>
+  <si>
+    <t>Precisa colocar as siglas nas caixinhas</t>
   </si>
 </sst>
 </file>
@@ -16145,8 +16160,8 @@
   <dimension ref="A1:I1484"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A302" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C309" sqref="C309"/>
+      <pane ySplit="6" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.28515625" defaultRowHeight="11.25"/>
@@ -16676,10 +16691,10 @@
         <v>2238</v>
       </c>
       <c r="E31" s="13" t="s">
-        <v>2614</v>
-      </c>
-      <c r="F31" s="13" t="s">
-        <v>3885</v>
+        <v>2238</v>
+      </c>
+      <c r="F31" s="78" t="s">
+        <v>3896</v>
       </c>
       <c r="I31" s="15"/>
     </row>
@@ -29284,11 +29299,11 @@
       <c r="D672" s="14" t="s">
         <v>2238</v>
       </c>
-      <c r="E672" s="95" t="s">
-        <v>2614</v>
-      </c>
-      <c r="F672" s="95" t="s">
-        <v>3885</v>
+      <c r="E672" s="13" t="s">
+        <v>2238</v>
+      </c>
+      <c r="F672" s="13" t="s">
+        <v>3892</v>
       </c>
       <c r="I672" s="15"/>
     </row>
@@ -29323,10 +29338,10 @@
       <c r="D674" s="14" t="s">
         <v>2238</v>
       </c>
-      <c r="E674" s="95" t="s">
+      <c r="E674" s="13" t="s">
         <v>2614</v>
       </c>
-      <c r="F674" s="95" t="s">
+      <c r="F674" s="13" t="s">
         <v>3885</v>
       </c>
       <c r="I674" s="15"/>
@@ -40581,10 +40596,7 @@
         <v>2238</v>
       </c>
       <c r="E1255" s="13" t="s">
-        <v>2614</v>
-      </c>
-      <c r="F1255" s="13" t="s">
-        <v>3885</v>
+        <v>2238</v>
       </c>
       <c r="I1255" s="15"/>
     </row>
@@ -40602,10 +40614,7 @@
         <v>2238</v>
       </c>
       <c r="E1256" s="13" t="s">
-        <v>2614</v>
-      </c>
-      <c r="F1256" s="13" t="s">
-        <v>3885</v>
+        <v>2238</v>
       </c>
       <c r="I1256" s="15"/>
     </row>
@@ -40623,10 +40632,7 @@
         <v>2238</v>
       </c>
       <c r="E1257" s="13" t="s">
-        <v>2614</v>
-      </c>
-      <c r="F1257" s="13" t="s">
-        <v>3885</v>
+        <v>2238</v>
       </c>
       <c r="I1257" s="15"/>
     </row>
@@ -40644,10 +40650,7 @@
         <v>2238</v>
       </c>
       <c r="E1258" s="13" t="s">
-        <v>2614</v>
-      </c>
-      <c r="F1258" s="13" t="s">
-        <v>3885</v>
+        <v>2238</v>
       </c>
       <c r="I1258" s="15"/>
     </row>
@@ -40665,10 +40668,10 @@
         <v>2238</v>
       </c>
       <c r="E1259" s="13" t="s">
-        <v>2614</v>
+        <v>2238</v>
       </c>
       <c r="F1259" s="13" t="s">
-        <v>3885</v>
+        <v>3893</v>
       </c>
       <c r="I1259" s="15"/>
     </row>
@@ -40686,10 +40689,10 @@
         <v>2238</v>
       </c>
       <c r="E1260" s="13" t="s">
-        <v>2614</v>
-      </c>
-      <c r="F1260" s="13" t="s">
-        <v>3885</v>
+        <v>2238</v>
+      </c>
+      <c r="F1260" s="78" t="s">
+        <v>3894</v>
       </c>
       <c r="I1260" s="15"/>
     </row>
@@ -40707,10 +40710,7 @@
         <v>2238</v>
       </c>
       <c r="E1261" s="13" t="s">
-        <v>2614</v>
-      </c>
-      <c r="F1261" s="13" t="s">
-        <v>3885</v>
+        <v>2238</v>
       </c>
       <c r="I1261" s="15"/>
     </row>
@@ -40788,10 +40788,7 @@
         <v>2238</v>
       </c>
       <c r="E1265" s="13" t="s">
-        <v>2614</v>
-      </c>
-      <c r="F1265" s="13" t="s">
-        <v>3885</v>
+        <v>2238</v>
       </c>
       <c r="I1265" s="15"/>
     </row>
@@ -40827,7 +40824,7 @@
         <v>2238</v>
       </c>
       <c r="E1267" s="13" t="s">
-        <v>2614</v>
+        <v>2238</v>
       </c>
       <c r="F1267" s="13" t="s">
         <v>3885</v>
@@ -40869,10 +40866,10 @@
         <v>2238</v>
       </c>
       <c r="E1269" s="13" t="s">
-        <v>2614</v>
-      </c>
-      <c r="F1269" s="13" t="s">
-        <v>3885</v>
+        <v>2238</v>
+      </c>
+      <c r="F1269" s="78" t="s">
+        <v>3895</v>
       </c>
       <c r="I1269" s="15"/>
     </row>
@@ -40890,10 +40887,7 @@
         <v>2238</v>
       </c>
       <c r="E1270" s="13" t="s">
-        <v>2614</v>
-      </c>
-      <c r="F1270" s="13" t="s">
-        <v>3885</v>
+        <v>2238</v>
       </c>
       <c r="I1270" s="15"/>
     </row>

</xml_diff>